<commit_message>
Add files permission-control functionality (client)
</commit_message>
<xml_diff>
--- a/טבלאות db.xlsx
+++ b/טבלאות db.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Esther\studies\אחר\הפרויקט\github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Esther\studies\אחר\הפרויקט\github2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -230,23 +230,32 @@
     <t>***</t>
   </si>
   <si>
-    <t>0- רק עו"ד</t>
-  </si>
-  <si>
-    <t>1- גם מי שהעלה</t>
-  </si>
-  <si>
-    <t>2- כולם</t>
-  </si>
-  <si>
     <t>פעולות</t>
+  </si>
+  <si>
+    <t>0- רק אתה</t>
+  </si>
+  <si>
+    <t>1- רק מי שהעלה את המסמך (דיפולטיבי)</t>
+  </si>
+  <si>
+    <t>2- רק הקונים</t>
+  </si>
+  <si>
+    <t>3- רק המוכרים</t>
+  </si>
+  <si>
+    <t>4- כל עו"ד וב"כ המשתתפים בתיק</t>
+  </si>
+  <si>
+    <t>5- כל המשתתפים בתיק</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +323,11 @@
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -389,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -424,6 +438,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,16 +751,6 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="טבלה14" displayName="טבלה14" ref="S18:S21" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="S18:S21"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="לינקים"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="טבלה15" displayName="טבלה15" ref="U18:U25" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="U18:U25"/>
   <tableColumns count="1">
@@ -750,7 +760,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="טבלה16" displayName="טבלה16" ref="V7:V13" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="V7:V13"/>
   <tableColumns count="1">
@@ -760,11 +770,21 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="טבלה17" displayName="טבלה17" ref="W18:W20" totalsRowShown="0">
   <autoFilter ref="W18:W20"/>
   <tableColumns count="1">
     <tableColumn id="1" name="ערים"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="טבלה14" displayName="טבלה14" ref="S19:S22" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="S19:S22"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="לינקים"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -821,8 +841,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="טבלה11" displayName="טבלה11" ref="Q18:Q21" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="Q18:Q21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="טבלה11" displayName="טבלה11" ref="Q19:Q22" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="Q19:Q22"/>
   <tableColumns count="1">
     <tableColumn id="1" name="פעולות לתיקים"/>
   </tableColumns>
@@ -831,8 +851,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="טבלה12" displayName="טבלה12" ref="R7:R16" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="R7:R16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="טבלה12" displayName="טבלה12" ref="R8:R17" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="R8:R17"/>
   <tableColumns count="1">
     <tableColumn id="1" name="תבניות פעולה"/>
   </tableColumns>
@@ -1116,7 +1136,7 @@
   <dimension ref="G1:W27"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1124,33 +1144,41 @@
     <col min="7" max="25" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="U1" t="s">
+    <row r="1" spans="7:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="7:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="N2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="U2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="7:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="7:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="N3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="U3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="7:22" x14ac:dyDescent="0.2">
-      <c r="U4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="S3" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="7:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="S4" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="7:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="S5" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="7:22" ht="15" x14ac:dyDescent="0.2">
       <c r="G6" s="1"/>
       <c r="H6" s="8" t="s">
         <v>49</v>
@@ -1162,8 +1190,8 @@
       <c r="P6" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="R6" s="15" t="s">
-        <v>62</v>
+      <c r="S6" s="20" t="s">
+        <v>74</v>
       </c>
       <c r="T6" s="15" t="s">
         <v>62</v>
@@ -1187,10 +1215,7 @@
         <v>5</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="R7" s="14" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="T7" s="14" t="s">
         <v>22</v>
@@ -1212,8 +1237,8 @@
       <c r="P8" t="s">
         <v>0</v>
       </c>
-      <c r="R8" t="s">
-        <v>0</v>
+      <c r="R8" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="T8" t="s">
         <v>0</v>
@@ -1237,7 +1262,7 @@
         <v>21</v>
       </c>
       <c r="R9" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T9" t="s">
         <v>17</v>
@@ -1263,7 +1288,7 @@
         <v>18</v>
       </c>
       <c r="R10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -1286,7 +1311,7 @@
         <v>12</v>
       </c>
       <c r="R11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S11" s="7" t="s">
         <v>51</v>
@@ -1309,7 +1334,7 @@
         <v>13</v>
       </c>
       <c r="R12" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="V12" t="s">
         <v>41</v>
@@ -1323,7 +1348,7 @@
         <v>16</v>
       </c>
       <c r="R13" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="V13" t="s">
         <v>40</v>
@@ -1337,7 +1362,7 @@
         <v>32</v>
       </c>
       <c r="R14" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="7:22" x14ac:dyDescent="0.2">
@@ -1345,26 +1370,27 @@
         <v>53</v>
       </c>
       <c r="R15" t="s">
-        <v>39</v>
-      </c>
-      <c r="S15" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="S15" s="6"/>
     </row>
     <row r="16" spans="7:22" x14ac:dyDescent="0.2">
       <c r="R16" t="s">
+        <v>39</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="7:23" x14ac:dyDescent="0.2">
+      <c r="R17" t="s">
         <v>54</v>
       </c>
-      <c r="S16" s="10" t="s">
+      <c r="S17" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="T16" s="11" t="s">
+      <c r="T17" s="11" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="7:23" x14ac:dyDescent="0.2">
-      <c r="S17" s="15" t="s">
-        <v>62</v>
       </c>
       <c r="U17" s="15" t="s">
         <v>62</v>
@@ -1380,11 +1406,8 @@
       <c r="I18" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="Q18" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="S18" s="14" t="s">
-        <v>45</v>
+      <c r="S18" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="U18" s="14" t="s">
         <v>23</v>
@@ -1400,11 +1423,11 @@
       <c r="I19" t="s">
         <v>0</v>
       </c>
-      <c r="Q19" t="s">
-        <v>0</v>
-      </c>
-      <c r="S19" t="s">
-        <v>0</v>
+      <c r="Q19" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="S19" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="U19" t="s">
         <v>0</v>
@@ -1421,10 +1444,10 @@
         <v>10</v>
       </c>
       <c r="Q20" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U20" t="s">
         <v>1</v>
@@ -1444,10 +1467,10 @@
         <v>57</v>
       </c>
       <c r="Q21" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="S21" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="U21" t="s">
         <v>25</v>
@@ -1459,6 +1482,12 @@
       </c>
       <c r="I22" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>15</v>
+      </c>
+      <c r="S22" t="s">
+        <v>31</v>
       </c>
       <c r="U22" t="s">
         <v>61</v>

</xml_diff>